<commit_message>
Added all drop-down and non-dropdown classes for all sites.
</commit_message>
<xml_diff>
--- a/src/main/resources/4autoinsurancequote.xlsx
+++ b/src/main/resources/4autoinsurancequote.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tayu\Code\Java_Workspace\MdaChecker\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32420F5E-FD1F-4D54-9155-EFA493EF2315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20ECB47-970D-4B06-BC05-4EDCB93845BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{B6EB72F0-64CA-4968-A2A3-D44D286F65C3}"/>
   </bookViews>
@@ -37,15 +37,9 @@
     <t>mdaTitleHomePage</t>
   </si>
   <si>
-    <t>mdaTextHomepage</t>
-  </si>
-  <si>
     <t>mdaTextHeader</t>
   </si>
   <si>
-    <t>MdaTitle</t>
-  </si>
-  <si>
     <t>mdaText</t>
   </si>
   <si>
@@ -55,9 +49,6 @@
     <t>pageTitleCurrentTab</t>
   </si>
   <si>
-    <t>pageTitlenewTab</t>
-  </si>
-  <si>
     <t>hasDropDown</t>
   </si>
   <si>
@@ -92,6 +83,15 @@
   </si>
   <si>
     <t>06457</t>
+  </si>
+  <si>
+    <t>mdaTextHomePage</t>
+  </si>
+  <si>
+    <t>pageTitleNewTab</t>
+  </si>
+  <si>
+    <t>mdaTitle</t>
   </si>
 </sst>
 </file>
@@ -447,7 +447,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,87 +461,87 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>99999</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>